<commit_message>
actualizacion de los axcel en assa
</commit_message>
<xml_diff>
--- a/DashboarJira/PlantillasExcel/Plantilla MTE-TEL-22 Assa.xlsx
+++ b/DashboarJira/PlantillasExcel/Plantilla MTE-TEL-22 Assa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\OneDrive\Documentos\GitHub\IndicadoresSDKJira\DashboarJira\PlantillasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66C383-C052-47E5-854A-5E50B8E028DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C878211F-7A10-498E-982A-F0E376B8401F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,13 +339,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="FF00A5D1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,111 +514,93 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -645,6 +627,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,6 +652,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00A5D1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1222,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AO54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:Q21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,187 +1266,187 @@
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="8"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="12"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="15"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="47"/>
     </row>
     <row r="7" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="18" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="50"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="44"/>
     </row>
     <row r="8" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="18" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="50"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="44"/>
     </row>
     <row r="9" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="42" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="18" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="48"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="44"/>
     </row>
     <row r="10" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="19" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="48"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="44"/>
     </row>
     <row r="11" spans="2:17" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="22"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="50"/>
     </row>
     <row r="12" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
@@ -1626,30 +1631,30 @@
       <c r="Q21" s="31"/>
     </row>
     <row r="22" spans="2:17" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="22"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="50"/>
     </row>
     <row r="23" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="32" t="s">
         <v>14</v>
       </c>
@@ -1668,760 +1673,692 @@
       <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="35" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="38" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="40"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
       <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="35" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
       <c r="Q26" s="6"/>
     </row>
     <row r="27" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="35" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="37"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="35" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
       <c r="Q28" s="6"/>
     </row>
     <row r="29" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
       <c r="Q30" s="6"/>
     </row>
     <row r="31" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="35" t="s">
+      <c r="C31" s="16"/>
+      <c r="D31" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="37"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="19"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="19"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="19"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="35" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="19"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
       <c r="Q35" s="6"/>
     </row>
     <row r="36" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="35" t="s">
+      <c r="C36" s="16"/>
+      <c r="D36" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="19"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
       <c r="Q36" s="6"/>
     </row>
     <row r="37" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="35" t="s">
+      <c r="C37" s="16"/>
+      <c r="D37" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="19"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
       <c r="Q37" s="6"/>
     </row>
     <row r="38" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="35" t="s">
+      <c r="C38" s="16"/>
+      <c r="D38" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="19"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
       <c r="Q38" s="6"/>
     </row>
     <row r="39" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="35" t="s">
+      <c r="C39" s="16"/>
+      <c r="D39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="19"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
       <c r="Q39" s="6"/>
     </row>
     <row r="40" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="38" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="40"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="22"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
       <c r="Q40" s="6"/>
     </row>
     <row r="41" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="16"/>
+      <c r="D41" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="19"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
       <c r="Q41" s="6"/>
     </row>
     <row r="42" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="35" t="s">
+      <c r="C42" s="16"/>
+      <c r="D42" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="19"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
       <c r="Q42" s="6"/>
     </row>
     <row r="43" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="38" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="22"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
       <c r="Q43" s="6"/>
     </row>
     <row r="44" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="35" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="19"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
       <c r="Q44" s="6"/>
-      <c r="AO44" s="41"/>
+      <c r="AO44" s="14"/>
     </row>
     <row r="45" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="35" t="s">
+      <c r="C45" s="16"/>
+      <c r="D45" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="19"/>
       <c r="K45" s="5"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
       <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="35" t="s">
+      <c r="C46" s="16"/>
+      <c r="D46" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="19"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
       <c r="Q46" s="6"/>
     </row>
     <row r="47" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="35" t="s">
+      <c r="C47" s="16"/>
+      <c r="D47" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="37"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="19"/>
       <c r="K47" s="5"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
       <c r="Q47" s="6"/>
     </row>
     <row r="48" spans="2:41" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="35" t="s">
+      <c r="C48" s="16"/>
+      <c r="D48" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="37"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="19"/>
       <c r="K48" s="5"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
       <c r="Q48" s="6"/>
     </row>
     <row r="49" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="35" t="s">
+      <c r="C49" s="16"/>
+      <c r="D49" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="37"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="19"/>
       <c r="K49" s="5"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
       <c r="Q49" s="6"/>
     </row>
     <row r="50" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="35" t="s">
+      <c r="C50" s="16"/>
+      <c r="D50" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="37"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="19"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
       <c r="Q50" s="6"/>
     </row>
     <row r="51" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="35" t="s">
+      <c r="C51" s="16"/>
+      <c r="D51" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="37"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="19"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
       <c r="Q51" s="6"/>
     </row>
     <row r="52" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="35" t="s">
+      <c r="C52" s="16"/>
+      <c r="D52" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="37"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="19"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
       <c r="Q52" s="6"/>
     </row>
     <row r="53" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="35" t="s">
+      <c r="C53" s="16"/>
+      <c r="D53" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="37"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="19"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
       <c r="Q53" s="6"/>
     </row>
     <row r="54" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="35" t="s">
+      <c r="C54" s="16"/>
+      <c r="D54" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="10"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="12"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:J54"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:J53"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:J48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:J36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q21"/>
-    <mergeCell ref="B22:Q22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:J23"/>
+  <mergeCells count="80">
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E3:P3"/>
-    <mergeCell ref="E6:Q6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -2433,6 +2370,73 @@
     <mergeCell ref="K8:Q8"/>
     <mergeCell ref="K9:Q9"/>
     <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q21"/>
+    <mergeCell ref="B22:Q22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:J36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:J54"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:J53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>